<commit_message>
need to finish GOMS test Update
updated Goms COMP needs to be done
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Evaluation/GOMS_COMP.xlsx
+++ b/Project supporting Artifacts/Evaluation/GOMS_COMP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikodem/Documents/GitHub/TUD-Group-Project/Project supporting Artifacts/Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8664E2-A6CC-FC43-B09D-78A252C0D5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048A407D-440B-FD4A-B70F-7863BFF78C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9320" yWindow="500" windowWidth="14280" windowHeight="16080" xr2:uid="{4FF5F388-14DE-5040-B071-95F76F7E24BA}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="232">
   <si>
     <t>Task</t>
   </si>
@@ -503,16 +503,7 @@
     <t>Use 'Date' widget to extract date components.</t>
   </si>
   <si>
-    <t>Python (min)</t>
-  </si>
-  <si>
-    <t>ORANGE (min)</t>
-  </si>
-  <si>
     <t>de.head()</t>
-  </si>
-  <si>
-    <t>Data Polish (min)</t>
   </si>
   <si>
     <t>Label encoding</t>
@@ -1210,7 +1201,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1225,338 +1216,161 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <f>Normalisation!C7</f>
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
-        <f>Normalisation!G7</f>
-        <v>8</v>
-      </c>
-      <c r="D2" s="2">
-        <f>Normalisation!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <f>'Missing Values'!C8</f>
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <f>'Missing Values'!G7</f>
-        <v>6</v>
-      </c>
-      <c r="D3" s="2">
-        <f>'Missing Values'!K7</f>
-        <v>7</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <f>'Outlier Removal'!C8</f>
-        <v>13</v>
-      </c>
-      <c r="C4" s="2">
-        <f>'Outlier Removal'!G7</f>
-        <v>14</v>
-      </c>
-      <c r="D4" s="2">
-        <f>'Outlier Removal'!K7</f>
-        <v>5</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="2">
-        <f>'Label encoding'!C7</f>
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <f>'Label encoding'!G7</f>
-        <v>6</v>
-      </c>
-      <c r="D5" s="2">
-        <f>'Label encoding'!K7</f>
-        <v>5</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" s="2">
-        <f>binning!C7</f>
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <f>binning!G7</f>
-        <v>6</v>
-      </c>
-      <c r="D6" s="2">
-        <f>binning!K7</f>
-        <v>5</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <f>'Change Column Type'!C7</f>
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
-        <f>'Change Column Type'!G7</f>
-        <v>8</v>
-      </c>
-      <c r="D7" s="2">
-        <f>'Change Column Type'!K7</f>
-        <v>5</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <f>'Rename Column'!C6</f>
-        <v>6</v>
-      </c>
-      <c r="C8" s="2">
-        <f>'Rename Column'!G6</f>
-        <v>6</v>
-      </c>
-      <c r="D8" s="2">
-        <f>'Rename Column'!K7</f>
-        <v>4</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <f>'Special Character Removal'!C7</f>
-        <v>8</v>
-      </c>
-      <c r="C9" s="2">
-        <f>'Special Character Removal'!G7</f>
-        <v>13</v>
-      </c>
-      <c r="D9" s="2">
-        <f>'Special Character Removal'!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
-        <f>'Trim Whitespace'!C7</f>
-        <v>7</v>
-      </c>
-      <c r="C10" s="2">
-        <f>'Trim Whitespace'!G7</f>
-        <v>6</v>
-      </c>
-      <c r="D10" s="2">
-        <f>'Trim Whitespace'!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
-        <f>'Replace Substrings'!C7</f>
-        <v>7</v>
-      </c>
-      <c r="C11" s="2">
-        <f>'Replace Substrings'!G7</f>
-        <v>7</v>
-      </c>
-      <c r="D11" s="2">
-        <f>'Replace Substrings'!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
-        <f>'Text Case'!C7</f>
-        <v>6</v>
-      </c>
-      <c r="C12" s="2">
-        <f>'Text Case'!G7</f>
-        <v>6</v>
-      </c>
-      <c r="D12" s="2">
-        <f>'Text Case'!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
-        <f>'Remove Stopwords'!C7</f>
-        <v>11</v>
-      </c>
-      <c r="C13" s="2">
-        <f>'Remove Stopwords'!G7</f>
-        <v>7</v>
-      </c>
-      <c r="D13" s="2">
-        <f>'Remove Stopwords'!K7</f>
-        <v>5</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
-        <f>'Collapse Rare Categories'!C8</f>
-        <v>13</v>
-      </c>
-      <c r="C14" s="2">
-        <f>'Collapse Rare Categories'!G8</f>
-        <v>9</v>
-      </c>
-      <c r="D14" s="2">
-        <f>'Collapse Rare Categories'!K7</f>
-        <v>7</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
-        <f>Tokenization!C7</f>
-        <v>7</v>
-      </c>
-      <c r="C15" s="2">
-        <f>Tokenization!G7</f>
-        <v>7</v>
-      </c>
-      <c r="D15" s="2">
-        <f>Tokenization!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <f>'Regex (Regular Expressions)'!C7</f>
-        <v>12</v>
-      </c>
-      <c r="C16" s="2">
-        <f>'Regex (Regular Expressions)'!G7</f>
-        <v>7</v>
-      </c>
-      <c r="D16" s="2">
-        <f>'Regex (Regular Expressions)'!K7</f>
-        <v>5</v>
-      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
-        <f>'Datetime Components'!C8</f>
-        <v>10</v>
-      </c>
-      <c r="C17" s="2">
-        <f>'Datetime Components'!G7</f>
-        <v>6</v>
-      </c>
-      <c r="D17" s="2">
-        <f>'Datetime Components'!K7</f>
-        <v>6</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" s="2">
-        <f>'Remove Duplicates'!C7</f>
-        <v>7</v>
-      </c>
-      <c r="C18" s="2">
-        <f>'Remove Duplicates'!G7</f>
-        <v>7</v>
-      </c>
-      <c r="D18" s="2">
-        <f>'Remove Duplicates'!K7</f>
-        <v>4</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="1">
-        <f>SUM(B2:B18)</f>
-        <v>135</v>
-      </c>
-      <c r="C19" s="1">
-        <f>SUM(C2:C18)</f>
-        <v>129</v>
-      </c>
-      <c r="D19" s="1">
-        <f>SUM(D2:D18)</f>
-        <v>94</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1">
-        <f>B19/60</f>
-        <v>2.25</v>
-      </c>
-      <c r="C20" s="1">
-        <f>C19/60</f>
-        <v>2.15</v>
-      </c>
-      <c r="D20" s="1">
-        <f>D19/60</f>
-        <v>1.5666666666666667</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -1656,7 +1470,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -1679,13 +1493,13 @@
         <v>122</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -1714,7 +1528,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -1743,7 +1557,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -1858,18 +1672,18 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>127</v>
@@ -1881,13 +1695,13 @@
         <v>128</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -1916,7 +1730,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -1927,7 +1741,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>41</v>
@@ -1945,7 +1759,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2060,7 +1874,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2083,13 +1897,13 @@
         <v>132</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -2118,7 +1932,7 @@
         <v>25</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2147,7 +1961,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2263,7 +2077,7 @@
         <v>25</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -2286,13 +2100,13 @@
         <v>135</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2321,7 +2135,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2350,7 +2164,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2464,7 +2278,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2487,13 +2301,13 @@
         <v>138</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -2522,7 +2336,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2551,7 +2365,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -2666,7 +2480,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2689,13 +2503,13 @@
         <v>141</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -2724,7 +2538,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="108" x14ac:dyDescent="0.2">
@@ -2753,7 +2567,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="36" x14ac:dyDescent="0.2">
@@ -2902,7 +2716,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -2925,13 +2739,13 @@
         <v>138</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -2960,7 +2774,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -2989,7 +2803,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -3104,7 +2918,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -3112,7 +2926,7 @@
         <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>84</v>
@@ -3127,13 +2941,13 @@
         <v>144</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -3162,7 +2976,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -3191,7 +3005,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -3306,7 +3120,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="36" x14ac:dyDescent="0.2">
@@ -3317,7 +3131,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>146</v>
@@ -3329,13 +3143,13 @@
         <v>147</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -3364,7 +3178,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -3393,7 +3207,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="36" x14ac:dyDescent="0.2">
@@ -3538,56 +3352,56 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="36" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="K4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>112</v>
@@ -3596,7 +3410,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="36" x14ac:dyDescent="0.2">
@@ -3607,7 +3421,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>41</v>
@@ -3625,7 +3439,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -3741,7 +3555,7 @@
         <v>25</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -3752,7 +3566,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>117</v>
@@ -3764,13 +3578,13 @@
         <v>118</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="198" x14ac:dyDescent="0.2">
@@ -3781,7 +3595,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>112</v>
@@ -3799,7 +3613,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="108" x14ac:dyDescent="0.2">
@@ -3810,7 +3624,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>41</v>
@@ -3828,7 +3642,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.2">
@@ -3946,7 +3760,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -3970,13 +3784,13 @@
         <v>95</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>103</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -4006,7 +3820,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -4036,7 +3850,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -4169,7 +3983,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -4192,13 +4006,13 @@
         <v>101</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -4227,7 +4041,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -4256,7 +4070,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="36" x14ac:dyDescent="0.2">
@@ -4383,56 +4197,56 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="198" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>112</v>
@@ -4441,7 +4255,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="126" x14ac:dyDescent="0.2">
@@ -4452,7 +4266,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>41</v>
@@ -4470,7 +4284,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.2">
@@ -4599,56 +4413,56 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="126" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="144" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>112</v>
@@ -4657,7 +4471,7 @@
         <v>25</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="108" x14ac:dyDescent="0.2">
@@ -4668,7 +4482,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>41</v>
@@ -4677,7 +4491,7 @@
         <v>29</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>41</v>
@@ -4686,7 +4500,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.2">
@@ -4800,7 +4614,7 @@
         <v>25</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -4823,13 +4637,13 @@
         <v>114</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -4858,7 +4672,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -4887,7 +4701,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">
@@ -5002,7 +4816,7 @@
         <v>29</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="72" x14ac:dyDescent="0.2">
@@ -5025,13 +4839,13 @@
         <v>108</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="54" x14ac:dyDescent="0.2">
@@ -5060,7 +4874,7 @@
         <v>29</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="36" x14ac:dyDescent="0.2">
@@ -5084,7 +4898,7 @@
         <v>29</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="17" x14ac:dyDescent="0.2">

</xml_diff>